<commit_message>
Changes for UI automation scripts and new version of  chrome driver added
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rijsanyal/Documents/Track Change Assignment/AmazonTestAutomation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570081D4-612D-1E4F-B8CE-74FECD4B9823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D168C0-FDCF-E54E-A635-3C7581A05695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" activeTab="4" xr2:uid="{28FFF262-0E59-EF46-BCC3-4CA21038B38D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{28FFF262-0E59-EF46-BCC3-4CA21038B38D}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Details" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>SAMPLE DATA 1</t>
   </si>
@@ -52,112 +52,124 @@
     <t>RANK</t>
   </si>
   <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>FULL NAME</t>
+  </si>
+  <si>
+    <t>MOBILE NO</t>
+  </si>
+  <si>
+    <t>PINCODE</t>
+  </si>
+  <si>
+    <t>HOUSE DETAILS</t>
+  </si>
+  <si>
+    <t>AREA DETAILS</t>
+  </si>
+  <si>
+    <t>LANDMARK</t>
+  </si>
+  <si>
+    <t>TOWN</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>Salt Lake City, Sector-1</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>USERDATA1</t>
+  </si>
+  <si>
+    <t>USERDATA2</t>
+  </si>
+  <si>
+    <t>USERDATA3</t>
+  </si>
+  <si>
+    <t>SECTION_NAME</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>Alexa</t>
+  </si>
+  <si>
+    <t>Kutchina</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Home &amp; Kitchen</t>
+  </si>
+  <si>
+    <t>Amazon Devices</t>
+  </si>
+  <si>
+    <t>CREDENTIALS</t>
+  </si>
+  <si>
+    <t>EMAIL ID</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>USERDATA</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Clothing &amp; Accessories</t>
+  </si>
+  <si>
+    <t>realme</t>
+  </si>
+  <si>
+    <t>Logitech B100</t>
+  </si>
+  <si>
+    <t>Shreya</t>
+  </si>
+  <si>
+    <t>8496232494</t>
+  </si>
+  <si>
+    <t>700091</t>
+  </si>
+  <si>
+    <t>IA 100</t>
+  </si>
+  <si>
+    <t>Bags, Wallets and Luggage</t>
+  </si>
+  <si>
     <t>#8</t>
   </si>
   <si>
-    <t>Bags, Wallets and Luggage</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>FULL NAME</t>
-  </si>
-  <si>
-    <t>MOBILE NO</t>
-  </si>
-  <si>
-    <t>PINCODE</t>
-  </si>
-  <si>
-    <t>HOUSE DETAILS</t>
-  </si>
-  <si>
-    <t>AREA DETAILS</t>
-  </si>
-  <si>
-    <t>LANDMARK</t>
-  </si>
-  <si>
-    <t>TOWN</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>Rijul Sanyal</t>
-  </si>
-  <si>
-    <t>AE 51</t>
-  </si>
-  <si>
-    <t>Salt Lake City, Sector-1</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>West Bengal</t>
-  </si>
-  <si>
-    <t>USERDATA1</t>
-  </si>
-  <si>
-    <t>USERDATA2</t>
-  </si>
-  <si>
-    <t>USERDATA3</t>
-  </si>
-  <si>
-    <t>SECTION_NAME</t>
-  </si>
-  <si>
-    <t>PRODUCT_NAME</t>
-  </si>
-  <si>
-    <t>Alexa</t>
-  </si>
-  <si>
-    <t>Kutchina</t>
-  </si>
-  <si>
-    <t>Airdopes 800</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Home &amp; Kitchen</t>
-  </si>
-  <si>
-    <t>Amazon Devices</t>
-  </si>
-  <si>
-    <t>CREDENTIALS</t>
-  </si>
-  <si>
-    <t>EMAIL ID</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>rijsanyal@deloitte.com</t>
-  </si>
-  <si>
-    <t>Hashed_1305</t>
-  </si>
-  <si>
-    <t>USERDATA</t>
-  </si>
-  <si>
-    <t>SEARCH</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>8083789781</t>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>Amazon Fashion</t>
   </si>
 </sst>
 </file>
@@ -558,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4647A6-0D07-224C-A574-7D9B6F1F4400}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -571,52 +583,58 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EBAA9DCA-C8C7-0448-92EE-9EFEE3015B7B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459EA0B8-3014-5C46-8FFC-94FCD03D9883}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="280" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -626,10 +644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904FD775-545E-3146-9A5D-BADB14B69626}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="332" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -641,43 +659,51 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -702,15 +728,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -722,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8BE3-AE4D-DA4C-9590-84E685A07AE1}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="218" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -738,70 +764,67 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4">
-        <v>700064</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5678C6FB-DB0D-F74A-B85C-E26A188C4F54}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="316" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -824,13 +847,29 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{170F0786-5DC3-034F-8149-1677709D6BA8}">
+      <formula1>"Amazon Launchpad,Home Improvement,Clothing &amp; Accessories"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{07FD9D7E-BF3E-F947-A3B6-45D5E3391435}">
+      <formula1>"#1,#2,#3,#4,#5,#6,#7,#8,#9,#10"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes for adding new Excel helper to read all data from excel Added config java file instead of older config.properties
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rijsanyal/Documents/Track Change Assignment/AmazonTestAutomation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D168C0-FDCF-E54E-A635-3C7581A05695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F08D1A0-BB74-E84F-8F94-2ED044CEEEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{28FFF262-0E59-EF46-BCC3-4CA21038B38D}"/>
   </bookViews>
@@ -41,13 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
-  <si>
-    <t>SAMPLE DATA 1</t>
-  </si>
-  <si>
-    <t>BEST SELLER CATEGORY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>RANK</t>
   </si>
@@ -55,21 +49,9 @@
     <t>ADDRESS</t>
   </si>
   <si>
-    <t>FULL NAME</t>
-  </si>
-  <si>
-    <t>MOBILE NO</t>
-  </si>
-  <si>
     <t>PINCODE</t>
   </si>
   <si>
-    <t>HOUSE DETAILS</t>
-  </si>
-  <si>
-    <t>AREA DETAILS</t>
-  </si>
-  <si>
     <t>LANDMARK</t>
   </si>
   <si>
@@ -170,13 +152,100 @@
   </si>
   <si>
     <t>Amazon Fashion</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>6574980764</t>
+  </si>
+  <si>
+    <t>110004</t>
+  </si>
+  <si>
+    <t>RB Avenue</t>
+  </si>
+  <si>
+    <t>Deshpande Villa</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Ashwin</t>
+  </si>
+  <si>
+    <t>Chirag</t>
+  </si>
+  <si>
+    <t>9870657489</t>
+  </si>
+  <si>
+    <t>713205</t>
+  </si>
+  <si>
+    <t>Santipath</t>
+  </si>
+  <si>
+    <t>C-Zone</t>
+  </si>
+  <si>
+    <t>Durgapur</t>
+  </si>
+  <si>
+    <t>8676567412</t>
+  </si>
+  <si>
+    <t>742137</t>
+  </si>
+  <si>
+    <t>Dohalia</t>
+  </si>
+  <si>
+    <t>Murshidabad</t>
+  </si>
+  <si>
+    <t>Kalibari</t>
+  </si>
+  <si>
+    <t>COUNT_OF_DATA</t>
+  </si>
+  <si>
+    <t>FULL_NAME</t>
+  </si>
+  <si>
+    <t>MOBILE_NO</t>
+  </si>
+  <si>
+    <t>HOUSE_DETAILS</t>
+  </si>
+  <si>
+    <t>AREA_DETAILS</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>BEST_SELLER_CATEGORY</t>
+  </si>
+  <si>
+    <t>USERDATA4</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Nokia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,12 +266,15 @@
       <family val="3"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
       <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,20 +294,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,7 +642,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -583,17 +654,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -606,7 +678,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="280" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -616,107 +688,125 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904FD775-545E-3146-9A5D-BADB14B69626}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="332" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="239" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C46B8DC-5494-7F49-B999-472477340FF2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="261" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -728,94 +818,170 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8BE3-AE4D-DA4C-9590-84E685A07AE1}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="218" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="5" max="5" width="14" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="14" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -824,41 +990,41 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="316" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="20.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>40</v>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>39</v>
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -871,5 +1037,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates regarding xpath fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rijsanyal/Documents/Track Change Assignment/AmazonTestAutomation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F08D1A0-BB74-E84F-8F94-2ED044CEEEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC76F0E-4267-E042-86B6-4997B4B9A8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{28FFF262-0E59-EF46-BCC3-4CA21038B38D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>RANK</t>
   </si>
@@ -235,10 +235,16 @@
     <t>USERDATA4</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Nokia</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>USERDATA5</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -642,7 +648,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -717,10 +723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904FD775-545E-3146-9A5D-BADB14B69626}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="239" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -746,7 +752,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -756,10 +762,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -778,10 +784,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -793,6 +799,17 @@
       </c>
       <c r="D6" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +848,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>